<commit_message>
slide 6 tooltip width and adjust breakpoints for small desktops
</commit_message>
<xml_diff>
--- a/data/ClusterIncomes.xlsx
+++ b/data/ClusterIncomes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30960" windowHeight="18580"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -184,8 +184,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -680,15 +680,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -702,12 +698,16 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1053,55 +1053,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="4"/>
-    <col min="3" max="4" width="15.6640625" style="5"/>
-    <col min="5" max="10" width="15.6640625" style="8"/>
-    <col min="11" max="12" width="15.6640625" style="6"/>
-    <col min="13" max="16384" width="15.6640625" style="4"/>
+    <col min="1" max="1" width="75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3"/>
+    <col min="3" max="4" width="15.6640625" style="4"/>
+    <col min="5" max="10" width="15.6640625" style="6"/>
+    <col min="11" max="12" width="15.6640625" style="13"/>
+    <col min="13" max="16384" width="15.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="60" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="60" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1118,28 +1116,28 @@
       <c r="D2" s="1">
         <v>168684.53</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>3.3300000000000001E-3</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>0.37703799999999998</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <v>9.9903999999999993E-2</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <v>6.3272000000000009E-2</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <v>2.7120999999999999E-2</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="5">
         <v>6.0946E-2</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="12">
         <v>688260.05</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="12">
         <v>1100000</v>
       </c>
     </row>
@@ -1156,28 +1154,28 @@
       <c r="D3" s="1">
         <v>90530.37</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>0.34201999999999999</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>0.314664</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>0.25492199999999998</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>0.163552</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>9.7240999999999994E-2</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="5">
         <v>7.5461E-2</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="12">
         <v>200464.09</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="12">
         <v>533750</v>
       </c>
     </row>
@@ -1194,28 +1192,28 @@
       <c r="D4" s="1">
         <v>130970.81</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0.95542000000000005</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>0.43346400000000002</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>0.27760400000000002</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>0.17219200000000001</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>8.9460999999999999E-2</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>8.6960999999999997E-2</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="12">
         <v>200731.38</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="12">
         <v>657000</v>
       </c>
     </row>
@@ -1232,28 +1230,28 @@
       <c r="D5" s="1">
         <v>319681.59999999998</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>9.6100000000000005E-3</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>0.59913700000000003</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>0.15314900000000001</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>0.12640299999999999</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>2.0554000000000003E-2</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>3.8084E-2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="12">
         <v>714988.59</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="12">
         <v>1225000</v>
       </c>
     </row>
@@ -1270,28 +1268,28 @@
       <c r="D6" s="1">
         <v>255610.06</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>-5.1500000000000004E-2</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>0.31190600000000002</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>0.27752599999999999</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>0.25506799999999996</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <v>0.26949400000000001</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>3.3198999999999999E-2</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="12">
         <v>467081.33</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="12">
         <v>820000</v>
       </c>
     </row>
@@ -1308,28 +1306,28 @@
       <c r="D7" s="1">
         <v>171401.21</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>7.7210000000000001E-2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>0.341895</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>0.11838100000000001</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>0.10896599999999999</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <v>2.7886000000000001E-2</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <v>3.1899000000000004E-2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="12">
         <v>614756.55000000005</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="12">
         <v>1137500</v>
       </c>
     </row>
@@ -1346,28 +1344,28 @@
       <c r="D8" s="1">
         <v>120596.8</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>0.74485000000000001</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>0.286078</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>0.25282100000000002</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>0.12754200000000002</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <v>8.5599000000000008E-2</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <v>5.3281000000000002E-2</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="12">
         <v>185095.18</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="12">
         <v>673500</v>
       </c>
     </row>
@@ -1384,28 +1382,28 @@
       <c r="D9" s="1">
         <v>134389.54999999999</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>1.0966800000000001</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>0.27726699999999999</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>0.307031</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>0.18808800000000001</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <v>0.159354</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <v>9.4159000000000007E-2</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="12">
         <v>467749.55</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="12">
         <v>569500</v>
       </c>
     </row>
@@ -1422,28 +1420,28 @@
       <c r="D10" s="1">
         <v>102113.46</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>0.46750000000000003</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>0.43228700000000003</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>0.21937100000000001</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>0.12951399999999999</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <v>9.2604000000000006E-2</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <v>6.9968000000000002E-2</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="12">
         <v>360525.31</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="12">
         <v>692250</v>
       </c>
     </row>
@@ -1460,28 +1458,28 @@
       <c r="D11" s="1">
         <v>273758.40999999997</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>0.16818000000000002</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>0.71893299999999993</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>4.3437999999999997E-2</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>5.7485999999999995E-2</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <v>2.2636E-2</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <v>2.7486999999999998E-2</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="12">
         <v>553280.89</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="12">
         <v>852500</v>
       </c>
     </row>
@@ -1498,28 +1496,28 @@
       <c r="D12" s="1">
         <v>221989.75</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>-8.0310000000000006E-2</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>0.77168199999999998</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>4.7324000000000005E-2</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>5.3467000000000001E-2</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <v>2.2360999999999999E-2</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>2.4249999999999997E-2</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="12">
         <v>574663.73</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="12">
         <v>854375</v>
       </c>
     </row>
@@ -1536,28 +1534,28 @@
       <c r="D13" s="1">
         <v>250334.81</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>-7.980000000000001E-3</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>0.42821100000000001</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>6.5497E-2</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>8.4792000000000006E-2</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <v>1.508E-2</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>3.8128999999999996E-2</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="12">
         <v>633332.89</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="12">
         <v>930000</v>
       </c>
     </row>
@@ -1574,28 +1572,28 @@
       <c r="D14" s="1">
         <v>359349.14</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>6.565E-2</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>0.75506899999999999</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <v>7.1399000000000004E-2</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>9.4118999999999994E-2</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <v>0.33866999999999997</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>6.7793999999999993E-2</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="12">
         <v>676566.31</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="12">
         <v>1100000</v>
       </c>
     </row>
@@ -1612,28 +1610,28 @@
       <c r="D15" s="1">
         <v>191305.75</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>3.7199999999999998E-3</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <v>0.44426599999999999</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="5">
         <v>0.126307</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <v>0.101052</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="5">
         <v>5.7206E-2</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="5">
         <v>4.1352E-2</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="12">
         <v>506505.94</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="12">
         <v>852250</v>
       </c>
     </row>
@@ -1650,28 +1648,28 @@
       <c r="D16" s="1">
         <v>287604.12</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>0.1125</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <v>0.35095900000000002</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="5">
         <v>4.6849000000000002E-2</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>7.2789000000000006E-2</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="5">
         <v>1.8239000000000002E-2</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="5">
         <v>3.1600999999999997E-2</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="12">
         <v>788492.09</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="12">
         <v>1175000</v>
       </c>
     </row>
@@ -1688,28 +1686,28 @@
       <c r="D17" s="1">
         <v>203010.31</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>4.3380000000000002E-2</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>0.88365700000000003</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="5">
         <v>4.9423000000000002E-2</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <v>3.6282999999999996E-2</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="5">
         <v>3.8984999999999999E-2</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="5">
         <v>7.0479E-2</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="12">
         <v>438348.15</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="12">
         <v>714000</v>
       </c>
     </row>
@@ -1726,28 +1724,28 @@
       <c r="D18" s="1">
         <v>87748.45</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>-2.2869999999999998E-2</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <v>0.47958100000000004</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="5">
         <v>0.120726</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>0.15620200000000001</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="5">
         <v>7.0656999999999998E-2</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="5">
         <v>0.115962</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="12">
         <v>225188</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="12">
         <v>395000</v>
       </c>
     </row>
@@ -1764,28 +1762,28 @@
       <c r="D19" s="1">
         <v>91044.83</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>1.92E-3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>0.55056899999999998</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="5">
         <v>0.15115500000000001</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <v>0.15673199999999998</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="5">
         <v>7.8063999999999995E-2</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="5">
         <v>0.13318199999999999</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="12">
         <v>185763.39</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="12">
         <v>473700</v>
       </c>
     </row>
@@ -1802,28 +1800,28 @@
       <c r="D20" s="1">
         <v>82589.740000000005</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>-2.3029999999999998E-2</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="5">
         <v>0.53882099999999999</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="5">
         <v>9.7486000000000003E-2</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <v>0.15912800000000002</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="5">
         <v>0.15681599999999998</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="5">
         <v>0.11062699999999999</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="12">
         <v>170728.58</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="12">
         <v>267500</v>
       </c>
     </row>
@@ -1840,28 +1838,28 @@
       <c r="D21" s="1">
         <v>81493.440000000002</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>-0.11878999999999999</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="5">
         <v>0.69150999999999996</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="5">
         <v>9.6126000000000003E-2</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <v>0.13839299999999999</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="5">
         <v>0.141179</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="5">
         <v>0.15823999999999999</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="12">
         <v>191109.1</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="12">
         <v>346900</v>
       </c>
     </row>
@@ -1878,28 +1876,28 @@
       <c r="D22" s="1">
         <v>92847.360000000001</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>0.39433999999999997</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <v>0.46114600000000006</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="5">
         <v>0.234074</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <v>0.197072</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="5">
         <v>0.14255000000000001</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="5">
         <v>0.12524399999999999</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="12">
         <v>173735.55</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="12">
         <v>487000</v>
       </c>
     </row>
@@ -1916,28 +1914,28 @@
       <c r="D23" s="1">
         <v>87511.24</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>2.886E-2</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <v>0.60551999999999995</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="5">
         <v>0.18227699999999999</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="5">
         <v>0.18840499999999999</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="5">
         <v>0.123641</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="5">
         <v>0.16906600000000002</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="12">
         <v>169726.26</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="12">
         <v>400000</v>
       </c>
     </row>
@@ -1954,28 +1952,28 @@
       <c r="D24" s="1">
         <v>49758.85</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>-5.5490000000000005E-2</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <v>0.27385900000000002</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="5">
         <v>0.30388999999999999</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="5">
         <v>0.33347299999999996</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="5">
         <v>0.18299399999999999</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="5">
         <v>0.21331800000000001</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="12">
         <v>106914.18</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="12">
         <v>264900</v>
       </c>
     </row>
@@ -1992,28 +1990,28 @@
       <c r="D25" s="1">
         <v>97526</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>9.6210000000000004E-2</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <v>0.56146099999999999</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="5">
         <v>0.16182400000000002</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <v>0.152031</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="5">
         <v>0.114969</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="5">
         <v>0.18907800000000002</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="12">
         <v>189772.67</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="12">
         <v>399817</v>
       </c>
     </row>
@@ -2030,28 +2028,28 @@
       <c r="D26" s="1">
         <v>119966.21</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <v>0.38049999999999995</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <v>0.51677300000000004</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="5">
         <v>0.18389500000000003</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <v>0.147206</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="5">
         <v>0.10570700000000001</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="5">
         <v>8.4728999999999999E-2</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="12">
         <v>187099.82</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="12">
         <v>528000</v>
       </c>
     </row>
@@ -2068,28 +2066,28 @@
       <c r="D27" s="1">
         <v>189922.97</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <v>0.48908999999999997</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <v>0.54322400000000004</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="5">
         <v>0.152888</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <v>0.11757300000000001</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="5">
         <v>5.4649000000000003E-2</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="5">
         <v>5.6525999999999993E-2</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="12">
         <v>244566.19</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="12">
         <v>631500</v>
       </c>
     </row>
@@ -2106,28 +2104,28 @@
       <c r="D28" s="1">
         <v>123411.11</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <v>2.7403199999999996</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <v>0.25938600000000001</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="5">
         <v>0.62080199999999996</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <v>0.11995599999999999</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="5">
         <v>0.32671100000000003</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="5">
         <v>7.0944000000000007E-2</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="12">
         <v>131638.09</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="12">
         <v>826860</v>
       </c>
     </row>
@@ -2144,28 +2142,28 @@
       <c r="D29" s="1">
         <v>37432.92</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <v>-0.10012</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <v>0.23387899999999998</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="5">
         <v>0.37896000000000002</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="5">
         <v>0.47137000000000001</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="5">
         <v>0.21739</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="5">
         <v>0.18946399999999999</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="12">
         <v>97559.19</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="12">
         <v>209000</v>
       </c>
     </row>
@@ -2182,28 +2180,28 @@
       <c r="D30" s="1">
         <v>49128.72</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <v>-0.16653999999999999</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="5">
         <v>0.43078899999999998</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="5">
         <v>0.28384599999999999</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="5">
         <v>0.42878300000000003</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="5">
         <v>0.20785200000000001</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="5">
         <v>0.30712800000000001</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="12">
         <v>180284.04</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="12">
         <v>250000</v>
       </c>
     </row>
@@ -2220,28 +2218,28 @@
       <c r="D31" s="1">
         <v>37806.14</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <v>-0.15720000000000001</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="5">
         <v>0.24810300000000002</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="5">
         <v>0.30187599999999998</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="5">
         <v>0.37273600000000001</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="5">
         <v>0.13944200000000001</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="5">
         <v>0.29120099999999999</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="12">
         <v>113596.32</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="12">
         <v>213750</v>
       </c>
     </row>
@@ -2258,28 +2256,28 @@
       <c r="D32" s="1">
         <v>53861.19</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="5">
         <v>-3.5560000000000001E-2</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="5">
         <v>0.36240299999999998</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="5">
         <v>0.27660000000000001</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="5">
         <v>0.31646599999999997</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="5">
         <v>0.162859</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="5">
         <v>0.23252199999999998</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="12">
         <v>96790.75</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="12">
         <v>200000</v>
       </c>
     </row>
@@ -2296,28 +2294,28 @@
       <c r="D33" s="1">
         <v>59473.48</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <v>0.11882</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="5">
         <v>0.34143099999999998</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="5">
         <v>0.23897300000000002</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <v>0.24367899999999998</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="5">
         <v>0.131412</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="5">
         <v>0.201903</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="12">
         <v>119610.24000000001</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="12">
         <v>218000</v>
       </c>
     </row>
@@ -2334,28 +2332,28 @@
       <c r="D34" s="1">
         <v>60420.07</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <v>0.12019000000000001</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="5">
         <v>0.43112200000000001</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="5">
         <v>0.32957000000000003</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="5">
         <v>0.263465</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="5">
         <v>0.17585499999999998</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="5">
         <v>0.204013</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="12">
         <v>127027.41</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="12">
         <v>242500</v>
       </c>
     </row>
@@ -2372,28 +2370,28 @@
       <c r="D35" s="1">
         <v>77364.97</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="5">
         <v>-7.2220000000000006E-2</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="5">
         <v>0.47268500000000002</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="5">
         <v>0.15459699999999998</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="5">
         <v>0.18610399999999999</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="5">
         <v>0.12029400000000001</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J35" s="5">
         <v>0.18987899999999999</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="12">
         <v>140993.07999999999</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="12">
         <v>245000</v>
       </c>
     </row>
@@ -2410,28 +2408,28 @@
       <c r="D36" s="1">
         <v>83689.820000000007</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="5">
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="5">
         <v>0.44700899999999999</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="5">
         <v>0.158639</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="5">
         <v>0.142702</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="5">
         <v>8.3984000000000003E-2</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="5">
         <v>8.8180999999999995E-2</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="12">
         <v>233874.77</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="12">
         <v>324950</v>
       </c>
     </row>
@@ -2448,28 +2446,28 @@
       <c r="D37" s="1">
         <v>43391.25</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="5">
         <v>9.0569999999999998E-2</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="5">
         <v>0.153581</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="5">
         <v>0.47296199999999999</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="5">
         <v>0.49687100000000001</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="5">
         <v>0.21779000000000001</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="5">
         <v>0.25851400000000002</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="12">
         <v>133509.09</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="12">
         <v>175000</v>
       </c>
     </row>
@@ -2486,28 +2484,28 @@
       <c r="D38" s="1">
         <v>40753.379999999997</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <v>0.21443999999999999</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="5">
         <v>0.167104</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="5">
         <v>0.46179599999999998</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="5">
         <v>0.39676600000000001</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="5">
         <v>0.256295</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="5">
         <v>0.229406</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="12">
         <v>78254.5</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="12">
         <v>298900</v>
       </c>
     </row>
@@ -2524,28 +2522,28 @@
       <c r="D39" s="1">
         <v>44992.56</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>0.17806</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="5">
         <v>0.18041199999999999</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="5">
         <v>0.45090400000000003</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="5">
         <v>0.38367499999999999</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="5">
         <v>0.25920199999999999</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="5">
         <v>0.19937000000000002</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="12">
         <v>161773.85</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="12">
         <v>258000</v>
       </c>
     </row>
@@ -2562,33 +2560,33 @@
       <c r="D40" s="1">
         <v>41990</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="5">
         <v>-0.18140999999999999</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="5">
         <v>0.25053799999999998</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="5">
         <v>0.33457799999999999</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="5">
         <v>0.380996</v>
       </c>
-      <c r="I40" s="7">
+      <c r="I40" s="5">
         <v>0.19736300000000001</v>
       </c>
-      <c r="J40" s="7">
+      <c r="J40" s="5">
         <v>0.27116000000000001</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="12">
         <v>133608.65</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="12">
         <v>189000</v>
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mobile breakpoint = 600 for maps, slide 6, add google analytics
</commit_message>
<xml_diff>
--- a/data/ClusterIncomes.xlsx
+++ b/data/ClusterIncomes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30960" windowHeight="18580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31940" windowHeight="20260"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
-    <t>Cluster Number</t>
-  </si>
-  <si>
-    <t>Cluster Name</t>
-  </si>
-  <si>
     <t>Kalorama Heights, Adams Morgan, Lanier Heights</t>
   </si>
   <si>
@@ -144,37 +138,43 @@
     <t>Congress Heights, Bellevue, Washington Highlands</t>
   </si>
   <si>
-    <t>Change in Family Income, 2000 to 2008-12</t>
-  </si>
-  <si>
-    <t>Homeownership Rate, 2008-12</t>
-  </si>
-  <si>
-    <t>Percent Below Poverty, 2000</t>
-  </si>
-  <si>
-    <t>Percent Below Poverty, 2008-12</t>
-  </si>
-  <si>
-    <t>Unemployment Rate, 2000</t>
-  </si>
-  <si>
-    <t>Unemployment Rate, 2008-12</t>
-  </si>
-  <si>
-    <t>Median Sales Price of Single Family Home (2012$), 2012</t>
-  </si>
-  <si>
-    <t>Median Sales Price of Single Family Home (2012$), 2000</t>
-  </si>
-  <si>
-    <t>Average Family Income (2012$), 2008-12</t>
-  </si>
-  <si>
-    <t>Average Family Income (2012$), 2000</t>
-  </si>
-  <si>
     <t>Source: Neighborhood Change Database, 2000; American Community Survey, 2008–12; and DC real property data calculated by NeighborhoodInfo DC for DC Office of Planning neighborhood cluster boundaries.</t>
+  </si>
+  <si>
+    <t>Cluster name</t>
+  </si>
+  <si>
+    <t>Cluster number</t>
+  </si>
+  <si>
+    <t>Average family income ($2012), 2000</t>
+  </si>
+  <si>
+    <t>Average family income ($2012), 2008–12</t>
+  </si>
+  <si>
+    <t>Change in family income, 2000 to 2008–12</t>
+  </si>
+  <si>
+    <t>Homeownership rate, 2008–12</t>
+  </si>
+  <si>
+    <t>Percent below poverty level, 2000</t>
+  </si>
+  <si>
+    <t>Percent below poverty, 2008–12</t>
+  </si>
+  <si>
+    <t>Unemployment rate, 2000</t>
+  </si>
+  <si>
+    <t>Unemployment rate, 2008–12</t>
+  </si>
+  <si>
+    <t>Median sales price of single family home ($2012), 2000</t>
+  </si>
+  <si>
+    <t>Median sales price of single family home ($2012), 2012</t>
   </si>
 </sst>
 </file>
@@ -184,8 +184,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -685,29 +685,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1067,45 +1067,45 @@
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" ht="60" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" s="11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -2473,7 +2473,7 @@
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>